<commit_message>
Push from new laptop
</commit_message>
<xml_diff>
--- a/src/test/resources/campaigncreation.xlsx
+++ b/src/test/resources/campaigncreation.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\raj-projects\TalentAcquisition\src\test\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\selenium-intellij\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9270"/>
   </bookViews>
   <sheets>
     <sheet name="create" sheetId="1" r:id="rId1"/>
-    <sheet name="target" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="28">
   <si>
     <t>campaign name</t>
   </si>
@@ -39,27 +38,9 @@
     <t>Enddate</t>
   </si>
   <si>
-    <t xml:space="preserve">State </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Region </t>
-  </si>
-  <si>
-    <t>city</t>
-  </si>
-  <si>
-    <t>area</t>
-  </si>
-  <si>
     <t>medium</t>
   </si>
   <si>
-    <t>Allmedics</t>
-  </si>
-  <si>
-    <t>ALL</t>
-  </si>
-  <si>
     <t>startmonth</t>
   </si>
   <si>
@@ -72,77 +53,94 @@
     <t>endyear</t>
   </si>
   <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>ANDHRA PRADESH</t>
-  </si>
-  <si>
-    <t>Coastal Andhra</t>
-  </si>
-  <si>
-    <t>ACHANTA</t>
-  </si>
-  <si>
-    <t>NATHAM</t>
-  </si>
-  <si>
     <t>Offline</t>
   </si>
   <si>
     <t>venu</t>
   </si>
   <si>
-    <t>Jobroles</t>
-  </si>
-  <si>
-    <t>No Of Hires</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
-    <t>APPRENTICE</t>
-  </si>
-  <si>
-    <t>Iam creating campaign with Apprentice Jobs Position</t>
-  </si>
-  <si>
-    <t>hyderabad telanagana</t>
-  </si>
-  <si>
-    <t>MediMart</t>
-  </si>
-  <si>
     <t>Mart</t>
   </si>
   <si>
-    <t>CHHATTISGARH</t>
-  </si>
-  <si>
-    <t>Bilaspur</t>
-  </si>
-  <si>
-    <t>RAIGARH</t>
-  </si>
-  <si>
-    <t>raipur</t>
-  </si>
-  <si>
-    <t>Camp C</t>
-  </si>
-  <si>
-    <t>A003</t>
+    <t xml:space="preserve">MediKit </t>
+  </si>
+  <si>
+    <t>January</t>
+  </si>
+  <si>
+    <t>Time Bounds</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>social media</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sourcetype </t>
+  </si>
+  <si>
+    <t>Creating  Campaign with Multiple Roles</t>
+  </si>
+  <si>
+    <t>Location type</t>
+  </si>
+  <si>
+    <t>MyLocation</t>
+  </si>
+  <si>
+    <r>
+      <t>Share Venue Contact Info</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> </t>
+    </r>
+  </si>
+  <si>
+    <t>Venue</t>
+  </si>
+  <si>
+    <t>secunderabad</t>
+  </si>
+  <si>
+    <t>SALE</t>
+  </si>
+  <si>
+    <t>FestiveSale</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -171,11 +169,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -456,31 +455,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N15"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.44140625" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="24.6640625" customWidth="1"/>
-    <col min="4" max="4" width="19.109375" customWidth="1"/>
-    <col min="5" max="5" width="29.88671875" customWidth="1"/>
-    <col min="6" max="6" width="21" customWidth="1"/>
-    <col min="7" max="7" width="20.21875" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" customWidth="1"/>
-    <col min="9" max="9" width="28.109375" customWidth="1"/>
-    <col min="10" max="10" width="19" customWidth="1"/>
-    <col min="11" max="11" width="21.6640625" customWidth="1"/>
-    <col min="12" max="12" width="19.109375" customWidth="1"/>
-    <col min="13" max="13" width="17.21875" customWidth="1"/>
-    <col min="14" max="15" width="31.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.42578125" customWidth="1"/>
+    <col min="2" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.7109375" customWidth="1"/>
+    <col min="5" max="5" width="19.140625" customWidth="1"/>
+    <col min="6" max="6" width="29.85546875" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="20.28515625" customWidth="1"/>
+    <col min="9" max="9" width="21.85546875" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1"/>
+    <col min="12" max="12" width="42.85546875" customWidth="1"/>
+    <col min="13" max="13" width="29.42578125" customWidth="1"/>
+    <col min="14" max="14" width="21" customWidth="1"/>
+    <col min="15" max="15" width="43.85546875" customWidth="1"/>
+    <col min="16" max="16" width="31.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,236 +488,169 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" t="s">
+        <v>4</v>
+      </c>
+      <c r="K1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N1" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2">
+        <v>2026</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2">
+        <v>2026</v>
+      </c>
+      <c r="I2">
+        <v>15</v>
+      </c>
+      <c r="J2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>25</v>
+      </c>
+      <c r="M2" t="s">
+        <v>16</v>
+      </c>
+      <c r="N2" t="s">
+        <v>18</v>
+      </c>
+      <c r="O2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="s">
         <v>12</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I1" t="s">
-        <v>4</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="E3">
+        <v>2026</v>
+      </c>
+      <c r="F3">
         <v>5</v>
       </c>
-      <c r="K1" t="s">
-        <v>6</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="G3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H3">
+        <v>2026</v>
+      </c>
+      <c r="I3">
+        <v>20</v>
+      </c>
+      <c r="J3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K3" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>2025</v>
-      </c>
-      <c r="E2">
-        <v>30</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2">
-        <v>2025</v>
-      </c>
-      <c r="H2">
-        <v>1</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="M3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" t="s">
+      <c r="N3" t="s">
         <v>18</v>
       </c>
-      <c r="K2" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" t="s">
+      <c r="O3" t="s">
         <v>20</v>
       </c>
-      <c r="M2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3">
-        <v>2025</v>
-      </c>
-      <c r="E3">
-        <v>30</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3">
-        <v>2025</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" t="s">
-        <v>31</v>
-      </c>
-      <c r="J3" t="s">
-        <v>32</v>
-      </c>
-      <c r="K3" t="s">
-        <v>33</v>
-      </c>
-      <c r="L3" t="s">
-        <v>33</v>
-      </c>
-      <c r="M3" t="s">
-        <v>21</v>
-      </c>
-      <c r="N3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>2025</v>
-      </c>
-      <c r="E4" s="1">
-        <v>9</v>
-      </c>
-      <c r="F4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4">
-        <v>2025</v>
-      </c>
-      <c r="H4" s="1">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
-      <c r="L4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="63.33203125" customWidth="1"/>
-    <col min="2" max="2" width="27.77734375" customWidth="1"/>
-    <col min="3" max="3" width="51.5546875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>